<commit_message>
Worked on Milestone #3, adding placeholder elements to the DOM
</commit_message>
<xml_diff>
--- a/WD+P5+-+Template+for+acceptance+test+plan.xlsx
+++ b/WD+P5+-+Template+for+acceptance+test+plan.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E419C13-3B78-46A2-A32D-D120A334C618}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Feature</t>
   </si>
@@ -35,6 +52,15 @@
   </si>
   <si>
     <t>OK / Error description</t>
+  </si>
+  <si>
+    <t>A product page showing details about the selected product.</t>
+  </si>
+  <si>
+    <t>Click on one of the products.</t>
+  </si>
+  <si>
+    <t>Opens a page in a new tab where the product is displayed with details about it. There are options for selecting colors and quantity also an "add to card button".</t>
   </si>
   <si>
     <t>...</t>
@@ -43,26 +69,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -71,7 +97,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,7 +107,13 @@
     </fill>
   </fills>
   <borders count="17">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -95,8 +127,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -106,6 +140,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -120,6 +155,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -134,6 +170,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -142,17 +179,22 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -161,9 +203,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -172,9 +216,11 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -189,8 +235,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -200,6 +248,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -214,6 +263,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -228,6 +278,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -242,8 +293,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -253,6 +306,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -267,6 +321,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -281,92 +336,81 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -556,26 +600,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.29"/>
-    <col customWidth="1" min="2" max="3" width="58.43"/>
-    <col customWidth="1" min="4" max="4" width="57.86"/>
-    <col customWidth="1" min="5" max="5" width="52.71"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="3" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="57.85546875" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" customHeight="1">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -590,9 +639,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="38.25">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -607,157 +656,163 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="78">
       <c r="A3" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="13">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="17"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="17"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="17"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="17"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="17"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="17"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="17"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Milestone #6 implemented and worked on the test plan
</commit_message>
<xml_diff>
--- a/WD+P5+-+Template+for+acceptance+test+plan.xlsx
+++ b/WD+P5+-+Template+for+acceptance+test+plan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25930"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E419C13-3B78-46A2-A32D-D120A334C618}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AD7373-5805-471A-AD2B-B4731C400DD9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Feature</t>
   </si>
@@ -57,20 +57,200 @@
     <t>A product page showing details about the selected product.</t>
   </si>
   <si>
-    <t>Click on one of the products.</t>
-  </si>
-  <si>
-    <t>Opens a page in a new tab where the product is displayed with details about it. There are options for selecting colors and quantity also an "add to card button".</t>
-  </si>
-  <si>
-    <t>...</t>
+    <t>Click on one of the products in the homepage.</t>
+  </si>
+  <si>
+    <t>Opens a page in a new tab where the selected product is displayed with details about it. As well as the price of the product and options for selecting colors and quantity. There is also a "add to card button".</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">From the product page users will be able to
+select the required quantity and colour and then add the product to the cart. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Part 1/3</t>
+    </r>
+  </si>
+  <si>
+    <t>Click on the "Please, select a color" in the product page.</t>
+  </si>
+  <si>
+    <t>Opens a dropdown menu where user can choose the color.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">From the product page users will be able to
+select the required quantity and colour and then add the product to the cart. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Part 2/3</t>
+    </r>
+  </si>
+  <si>
+    <t>Click on the field dedicated to "Number of articles (1-100):"</t>
+  </si>
+  <si>
+    <t>User can type in numbers(only) or use the arrow keys to change the quantity of the product.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">From the product page users will be able to
+select the required quantity and colour and then add the product to the cart.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Part 3/3</t>
+    </r>
+  </si>
+  <si>
+    <t>Click on the "Add to cart button"</t>
+  </si>
+  <si>
+    <t>The product'll be saved in the cart with the choosen color and quantity. (If the user clicks the "Add to cart button" muliple times for the same color, the product should show up in the cart page only once but the quantity should be respective to the total items added to the cart.)</t>
+  </si>
+  <si>
+    <t>A cart page showing (dynamically) all products seleceted previously.</t>
+  </si>
+  <si>
+    <t>Open the cart page on a browser.</t>
+  </si>
+  <si>
+    <t>Displays the items that has been previously selected as well as the total price for the items(dynamycally).</t>
+  </si>
+  <si>
+    <t>User can modify the quantity or delete products completely from the cart.</t>
+  </si>
+  <si>
+    <t>Changing the field dedicated to "Qty:" or the "Delete" button.</t>
+  </si>
+  <si>
+    <t>The "Total" section updates respectively and in case clicking the "Delete" button the item also disappears from the list in the cart.</t>
+  </si>
+  <si>
+    <t>Leaving the cart page, should not remove the items from the cart.</t>
+  </si>
+  <si>
+    <t>Refreshing or changing the page.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">A form to be submitted in order to confirm the order.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Part 1/3</t>
+    </r>
+  </si>
+  <si>
+    <t>Filling the form correctly.</t>
+  </si>
+  <si>
+    <t>Display no error. "Order!" button is "clickable".</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">A form to be submitted in order to confirm the order.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Part 2/3</t>
+    </r>
+  </si>
+  <si>
+    <t>Filling the form incorrectly.</t>
+  </si>
+  <si>
+    <t>Display an error message, for example: "Please include an '@' in ther email address. 'mygmail.com' missing an '@' sign.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">A form to be submitted in order to confirm the order.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Part 3/3</t>
+    </r>
+  </si>
+  <si>
+    <t>Clicking the "Order!" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the form was filled correctly, opens conformation page and delete items from the cart. If not the error message will show under the form field with the incorrect information. </t>
+  </si>
+  <si>
+    <t>Confirmation page showing the user’s order number sent by the API.</t>
+  </si>
+  <si>
+    <t>Thanking the user for the order and displaying the confirmation number. This number must be not stored anywhere.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -91,6 +271,16 @@
       <sz val="14"/>
       <name val="Montserrat"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Montserrat"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -342,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -356,18 +546,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -391,6 +569,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,8 +811,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -640,177 +839,279 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="38.25">
-      <c r="A2" s="5">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="78">
-      <c r="A3" s="9">
+      <c r="E2" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="116.25">
+      <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="9">
+      <c r="E3" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="96.75">
+      <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="9">
+      <c r="B4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="96.75">
+      <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="9">
+      <c r="B5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="154.5">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.75">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="78">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57.75">
+      <c r="A9" s="19">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.75">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="78">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="96.75">
+      <c r="A12" s="19">
         <v>11</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
+      <c r="B12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="57.75">
+      <c r="A13" s="19">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21.75">
+      <c r="A14" s="19">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="1:5" ht="21.75">
+      <c r="A15" s="19">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:5" ht="21.75">
+      <c r="A16" s="19">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" ht="21.75">
+      <c r="A17" s="19">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Small refinements, save before refactoring some of the functions
</commit_message>
<xml_diff>
--- a/WD+P5+-+Template+for+acceptance+test+plan.xlsx
+++ b/WD+P5+-+Template+for+acceptance+test+plan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26019"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="196" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AD7373-5805-471A-AD2B-B4731C400DD9}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19CFC7A5-FD84-4CA4-9D1E-3D1518118E93}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Feature</t>
   </si>
@@ -51,7 +51,7 @@
     <t>Display all the products</t>
   </si>
   <si>
-    <t>OK / Error description</t>
+    <t>OK / Error description: "Error! Check if server is up and running"</t>
   </si>
   <si>
     <t>A product page showing details about the selected product.</t>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Opens a dropdown menu where user can choose the color.</t>
+  </si>
+  <si>
+    <t>OK / Error description</t>
   </si>
   <si>
     <r>
@@ -811,8 +814,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -886,7 +889,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="96.75">
@@ -894,16 +897,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="154.5">
@@ -911,16 +914,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="57.75">
@@ -928,16 +931,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="78">
@@ -945,16 +948,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57.75">
@@ -962,16 +965,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.75">
@@ -979,16 +982,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="78">
@@ -996,16 +999,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="96.75">
@@ -1013,16 +1016,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="57.75">
@@ -1030,16 +1033,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21.75">

</xml_diff>

<commit_message>
Added comments for functions and small adjustments
</commit_message>
<xml_diff>
--- a/WD+P5+-+Template+for+acceptance+test+plan.xlsx
+++ b/WD+P5+-+Template+for+acceptance+test+plan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26102"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="198" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19CFC7A5-FD84-4CA4-9D1E-3D1518118E93}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F66790B-8B6F-4BDB-A6C3-BC48F0692DAB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Feature</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Opens a page in a new tab where the selected product is displayed with details about it. As well as the price of the product and options for selecting colors and quantity. There is also a "add to card button".</t>
+  </si>
+  <si>
+    <t>OK / Product page is not avalible is server is not running.</t>
   </si>
   <si>
     <r>
@@ -89,7 +92,7 @@
     <t>Opens a dropdown menu where user can choose the color.</t>
   </si>
   <si>
-    <t>OK / Error description</t>
+    <t>OK / Error description: "Error! Check if server is up and running" / In case there is no color selected: "Product color has not been selected, please pick a color"</t>
   </si>
   <si>
     <r>
@@ -118,6 +121,9 @@
     <t>User can type in numbers(only) or use the arrow keys to change the quantity of the product.</t>
   </si>
   <si>
+    <t>OK / In case user trying to enter "0": "Cannot add "0" articles to the cart, please select a valid value"</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="14"/>
@@ -144,6 +150,9 @@
     <t>The product'll be saved in the cart with the choosen color and quantity. (If the user clicks the "Add to cart button" muliple times for the same color, the product should show up in the cart page only once but the quantity should be respective to the total items added to the cart.)</t>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
     <t>A cart page showing (dynamically) all products seleceted previously.</t>
   </si>
   <si>
@@ -162,10 +171,16 @@
     <t>The "Total" section updates respectively and in case clicking the "Delete" button the item also disappears from the list in the cart.</t>
   </si>
   <si>
+    <t>OK / This option is not avalible if the server is down.</t>
+  </si>
+  <si>
     <t>Leaving the cart page, should not remove the items from the cart.</t>
   </si>
   <si>
     <t>Refreshing or changing the page.</t>
+  </si>
+  <si>
+    <t>OK / Error description: "Error! Check if server is up and running" - If the server is down non of the selected products shown in the cart, however if the server is restored, refreshing the page will load the products from local storage.</t>
   </si>
   <si>
     <r>
@@ -183,14 +198,17 @@
         <color rgb="FF00B050"/>
         <rFont val="Montserrat"/>
       </rPr>
-      <t>Part 1/3</t>
+      <t>Part 1/2</t>
     </r>
   </si>
   <si>
-    <t>Filling the form correctly.</t>
-  </si>
-  <si>
-    <t>Display no error. "Order!" button is "clickable".</t>
+    <t>Filling the form.</t>
+  </si>
+  <si>
+    <t>Display no error message.</t>
+  </si>
+  <si>
+    <t>OK  / Display an error message, for example: "You have entered an invalid email format!"</t>
   </si>
   <si>
     <r>
@@ -208,39 +226,17 @@
         <color rgb="FF00B050"/>
         <rFont val="Montserrat"/>
       </rPr>
-      <t>Part 2/3</t>
+      <t>Part 2/2</t>
     </r>
   </si>
   <si>
-    <t>Filling the form incorrectly.</t>
-  </si>
-  <si>
-    <t>Display an error message, for example: "Please include an '@' in ther email address. 'mygmail.com' missing an '@' sign.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">A form to be submitted in order to confirm the order.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Part 3/3</t>
-    </r>
-  </si>
-  <si>
     <t>Clicking the "Order!" button.</t>
   </si>
   <si>
-    <t xml:space="preserve">If the form was filled correctly, opens conformation page and delete items from the cart. If not the error message will show under the form field with the incorrect information. </t>
+    <t>If the form was filled correctly, opens conformation page and delete items from the cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK /  If the form was filled incorrectly, error messages will show under each form field with incorrect information. </t>
   </si>
   <si>
     <t>Confirmation page showing the user’s order number sent by the API.</t>
@@ -812,10 +808,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -872,7 +868,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="96.75">
@@ -880,16 +876,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="96.75">
@@ -897,16 +893,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="154.5">
@@ -914,16 +910,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="57.75">
@@ -931,16 +927,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="78">
@@ -948,33 +944,33 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57.75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="135.75">
       <c r="A9" s="19">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.75">
@@ -982,68 +978,60 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="78">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="57.75">
       <c r="A11" s="19">
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="96.75">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57.75">
       <c r="A12" s="19">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="57.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21.75">
       <c r="A13" s="19">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>14</v>
-      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" ht="21.75">
       <c r="A14" s="19">
@@ -1072,14 +1060,12 @@
       <c r="D16" s="16"/>
       <c r="E16" s="18"/>
     </row>
-    <row r="17" spans="1:5" ht="21.75">
-      <c r="A17" s="19">
-        <v>16</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="18"/>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5"/>
@@ -1103,18 +1089,11 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Better variable names and error message
</commit_message>
<xml_diff>
--- a/WD+P5+-+Template+for+acceptance+test+plan.xlsx
+++ b/WD+P5+-+Template+for+acceptance+test+plan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26105"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="232" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F66790B-8B6F-4BDB-A6C3-BC48F0692DAB}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="11_91AA243A728A0FAC69A50D5BD225213D414BF00E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{976E7D2B-C8D8-4A72-8C5E-4DA42D09687A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -51,7 +51,7 @@
     <t>Display all the products</t>
   </si>
   <si>
-    <t>OK / Error description: "Error! Check if server is up and running"</t>
+    <t>OK / Error description: "503 - Service Unavailable"</t>
   </si>
   <si>
     <t>A product page showing details about the selected product.</t>
@@ -63,7 +63,7 @@
     <t>Opens a page in a new tab where the selected product is displayed with details about it. As well as the price of the product and options for selecting colors and quantity. There is also a "add to card button".</t>
   </si>
   <si>
-    <t>OK / Product page is not avalible is server is not running.</t>
+    <t>OK / Product page is not avalible if server is not running.</t>
   </si>
   <si>
     <r>
@@ -92,7 +92,7 @@
     <t>Opens a dropdown menu where user can choose the color.</t>
   </si>
   <si>
-    <t>OK / Error description: "Error! Check if server is up and running" / In case there is no color selected: "Product color has not been selected, please pick a color"</t>
+    <t>OK / Error description: "503 - Service Unavailable" / In case there is no color selected: "Product color has not been selected, please pick a color"</t>
   </si>
   <si>
     <r>
@@ -180,7 +180,7 @@
     <t>Refreshing or changing the page.</t>
   </si>
   <si>
-    <t>OK / Error description: "Error! Check if server is up and running" - If the server is down non of the selected products shown in the cart, however if the server is restored, refreshing the page will load the products from local storage.</t>
+    <t>OK / Error description: ""503 - Service Unavailable" - If the server is down non of the selected products shown in the cart, however if the server is restored, refreshing the page will load the products from local storage.</t>
   </si>
   <si>
     <r>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Thanking the user for the order and displaying the confirmation number. This number must be not stored anywhere.</t>
+  </si>
+  <si>
+    <t>OK / Error description: "Error! Check if server is up and running"</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -455,73 +458,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -531,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -545,49 +531,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -810,8 +784,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -838,263 +812,201 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="38.25">
-      <c r="A2" s="17">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="116.25">
-      <c r="A3" s="19">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="96.75">
-      <c r="A4" s="19">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="96.75">
-      <c r="A5" s="19">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="154.5">
-      <c r="A6" s="19">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="57.75">
-      <c r="A7" s="19">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="78">
-      <c r="A8" s="19">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="135.75">
-      <c r="A9" s="19">
+    <row r="9" spans="1:5" ht="116.25">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.75">
-      <c r="A10" s="19">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.75">
-      <c r="A11" s="19">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.75">
-      <c r="A12" s="19">
+      <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="21.75">
-      <c r="A13" s="19">
-        <v>12</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" spans="1:5" ht="21.75">
-      <c r="A14" s="19">
-        <v>13</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" spans="1:5" ht="21.75">
-      <c r="A15" s="19">
-        <v>14</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:5" ht="21.75">
-      <c r="A16" s="19">
-        <v>15</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-    </row>
+      <c r="E12" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75"/>
+    <row r="14" spans="1:5" ht="12.75"/>
+    <row r="15" spans="1:5" ht="12.75"/>
+    <row r="16" spans="1:5" ht="12.75"/>
+    <row r="17" ht="12.75"/>
+    <row r="18" ht="12.75"/>
+    <row r="19" ht="12.75"/>
+    <row r="20" ht="12.75"/>
+    <row r="21" ht="12.75"/>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>

</xml_diff>